<commit_message>
Modified belongs, grupos, instruments, musician and plays excel tables to include new rock groups data
</commit_message>
<xml_diff>
--- a/Archivos Excel/belongs.xlsx
+++ b/Archivos Excel/belongs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\SkyDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAA565D-4B65-451D-B684-BFCAE92696DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{114ED246-227B-498E-B5C2-92D2EED11963}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1BB78441-2EC4-44D6-B897-C4964439FD70}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>#John Coltrane´s Band ID: 270</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>#Reincidentes´s Band ID: 430</t>
+  </si>
+  <si>
+    <t>#The Rolling Stones's Band ID: 781</t>
+  </si>
+  <si>
+    <t>#ACDC's Band ID: 362</t>
   </si>
 </sst>
 </file>
@@ -54,12 +60,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -74,11 +86,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,165 +411,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21093448-8957-4543-BBBA-439F823C666C}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="3">
         <v>6166844</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="3">
         <v>270</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="1"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>5334423</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>270</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="3">
         <v>4628696</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="3">
         <v>270</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="3">
         <v>8484326</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="3">
         <v>270</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="3">
         <v>5427651</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="3">
         <v>270</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="3">
         <v>5392301</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="3">
         <v>110</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="3">
         <v>5264892</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="3">
         <v>110</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>9452841</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="3">
         <v>110</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>5672350</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="3">
         <v>110</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+      <c r="A12" s="3">
         <v>4136534</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="3">
         <v>430</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="1"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="3">
         <v>7376429</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="3">
         <v>430</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="3">
         <v>4949485</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="3">
         <v>430</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="3">
         <v>4949365</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="3">
         <v>430</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="3">
         <v>5453651</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="3">
         <v>430</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>8321941</v>
+      </c>
+      <c r="B18" s="5">
+        <v>781</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>7984074</v>
+      </c>
+      <c r="B19" s="5">
+        <v>781</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>7438203</v>
+      </c>
+      <c r="B20" s="5">
+        <v>781</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>4632752</v>
+      </c>
+      <c r="B21" s="5">
+        <v>781</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>8372185</v>
+      </c>
+      <c r="B23" s="5">
+        <v>362</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>3245623</v>
+      </c>
+      <c r="B24" s="5">
+        <v>362</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>3144134</v>
+      </c>
+      <c r="B25" s="5">
+        <v>362</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>4321561</v>
+      </c>
+      <c r="B26" s="5">
+        <v>362</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="D1:E5"/>
     <mergeCell ref="D7:E10"/>
     <mergeCell ref="D12:E16"/>
+    <mergeCell ref="D18:E21"/>
+    <mergeCell ref="D23:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified tables except the ones from opinion and buy of....
</commit_message>
<xml_diff>
--- a/Archivos Excel/belongs.xlsx
+++ b/Archivos Excel/belongs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sergio\Desktop\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DC0969-769F-40D3-BE08-095F2B600E74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3856EAEE-BE85-4FD2-B578-95CC929BC6BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{1BB78441-2EC4-44D6-B897-C4964439FD70}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -95,17 +96,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21093448-8957-4543-BBBA-439F823C666C}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,17 +431,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="2">
+      <c r="A1" s="1">
         <v>6166844</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>270</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="2"/>
       <c r="G1" t="str">
         <f>CONCATENATE($J$1, A1,$L$1,B1,$K$1)</f>
         <v>insert into belongs values(6166844,270);</v>
@@ -459,329 +457,344 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>5334423</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>270</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="G2" t="str">
         <f>CONCATENATE($J$1, A2,$L$1,B2,$K$1)</f>
         <v>insert into belongs values(5334423,270);</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>4628696</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>270</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="G3" t="str">
         <f>CONCATENATE($J$1, A3,$L$1,B3,$K$1)</f>
         <v>insert into belongs values(4628696,270);</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>8484326</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>270</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
       <c r="G4" t="str">
         <f>CONCATENATE($J$1, A4,$L$1,B4,$K$1)</f>
         <v>insert into belongs values(8484326,270);</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>5427651</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>270</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
       <c r="G5" t="str">
         <f>CONCATENATE($J$1, A5,$L$1,B5,$K$1)</f>
         <v>insert into belongs values(5427651,270);</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>5392301</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>110</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="1"/>
+      <c r="D7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="2"/>
       <c r="G7" t="str">
         <f>CONCATENATE($J$1, A7,$L$1,B7,$K$1)</f>
         <v>insert into belongs values(5392301,110);</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>5264892</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>110</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="G8" t="str">
         <f>CONCATENATE($J$1, A8,$L$1,B8,$K$1)</f>
         <v>insert into belongs values(5264892,110);</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>9452841</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>110</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="G9" t="str">
         <f>CONCATENATE($J$1, A9,$L$1,B9,$K$1)</f>
         <v>insert into belongs values(9452841,110);</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>5672350</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>110</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
       <c r="G10" t="str">
         <f>CONCATENATE($J$1, A10,$L$1,B10,$K$1)</f>
         <v>insert into belongs values(5672350,110);</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>4136534</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>430</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="2"/>
       <c r="G12" t="str">
         <f>CONCATENATE($J$1, A12,$L$1,B12,$K$1)</f>
         <v>insert into belongs values(4136534,430);</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>7376429</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>430</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="G13" t="str">
         <f>CONCATENATE($J$1, A13,$L$1,B13,$K$1)</f>
         <v>insert into belongs values(7376429,430);</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>4949485</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>430</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
       <c r="G14" t="str">
         <f>CONCATENATE($J$1, A14,$L$1,B14,$K$1)</f>
         <v>insert into belongs values(4949485,430);</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>4949365</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>430</v>
       </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
       <c r="G15" t="str">
         <f>CONCATENATE($J$1, A15,$L$1,B15,$K$1)</f>
         <v>insert into belongs values(4949365,430);</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>5453651</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>430</v>
       </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
       <c r="G16" t="str">
         <f>CONCATENATE($J$1, A16,$L$1,B16,$K$1)</f>
         <v>insert into belongs values(5453651,430);</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="3">
         <v>8321941</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="4">
         <v>781</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="2"/>
       <c r="G18" t="str">
         <f>CONCATENATE($J$1, A18,$L$1,B18,$K$1)</f>
         <v>insert into belongs values(8321941,781);</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="3">
         <v>7984074</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="4">
         <v>781</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="G19" t="str">
         <f>CONCATENATE($J$1, A19,$L$1,B19,$K$1)</f>
         <v>insert into belongs values(7984074,781);</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="3">
         <v>7438203</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="4">
         <v>781</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
       <c r="G20" t="str">
         <f>CONCATENATE($J$1, A20,$L$1,B20,$K$1)</f>
         <v>insert into belongs values(7438203,781);</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="3">
         <v>4632752</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="4">
         <v>781</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
       <c r="G21" t="str">
         <f>CONCATENATE($J$1, A21,$L$1,B21,$K$1)</f>
         <v>insert into belongs values(4632752,781);</v>
       </c>
     </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+    </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="3">
         <v>8372185</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="4">
         <v>362</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E23" s="5"/>
+      <c r="E23" s="2"/>
       <c r="G23" t="str">
         <f>CONCATENATE($J$1, A23,$L$1,B23,$K$1)</f>
         <v>insert into belongs values(8372185,362);</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="3">
         <v>3245623</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="4">
         <v>362</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
       <c r="G24" t="str">
         <f>CONCATENATE($J$1, A24,$L$1,B24,$K$1)</f>
         <v>insert into belongs values(3245623,362);</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="3">
         <v>3144134</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="4">
         <v>362</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
       <c r="G25" t="str">
         <f>CONCATENATE($J$1, A25,$L$1,B25,$K$1)</f>
         <v>insert into belongs values(3144134,362);</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="3">
         <v>4321561</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="4">
         <v>362</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
       <c r="G26" t="str">
         <f>CONCATENATE($J$1, A26,$L$1,B26,$K$1)</f>
         <v>insert into belongs values(4321561,362);</v>

</xml_diff>